<commit_message>
First working count down
</commit_message>
<xml_diff>
--- a/lookup_calc.xlsx
+++ b/lookup_calc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Look-up 1" sheetId="1" r:id="rId1"/>
@@ -67,8 +67,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -85,15 +87,17 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -425,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1108,172 +1112,177 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1">
         <v>0</v>
       </c>
       <c r="B1">
         <v>80</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="3">
         <f>B1^(2/3)</f>
         <v>18.566355334451107</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>90</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <f t="shared" ref="C2:C13" si="0">B2^(2/3)</f>
         <v>20.082988502465078</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>100</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <f t="shared" si="0"/>
         <v>21.544346900318843</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>110</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <f t="shared" si="0"/>
         <v>22.957704246655549</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>120</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <f t="shared" si="0"/>
         <v>24.328807982293593</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="E5">
+        <f>B5-80</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>130</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <f t="shared" si="0"/>
         <v>25.662299438731413</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>140</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="3">
         <f t="shared" si="0"/>
         <v>26.961994997758488</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>150</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="3">
         <f t="shared" si="0"/>
         <v>28.231080866430847</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>160</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <f t="shared" si="0"/>
         <v>29.472251989123087</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>170</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="3">
         <f t="shared" si="0"/>
         <v>30.687813601627905</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <v>180</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="3">
         <f t="shared" si="0"/>
         <v>31.879757075478334</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
         <v>190</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="3">
         <f t="shared" si="0"/>
         <v>33.049817624300402</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <v>200</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="3">
         <f t="shared" si="0"/>
         <v>34.19951893353393</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>